<commit_message>
ultima alteração á proposta (em princípio)
</commit_message>
<xml_diff>
--- a/Proposta Projeto/CalendarizaçãoProjeto.xlsx
+++ b/Proposta Projeto/CalendarizaçãoProjeto.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Desktop\New folder\PDS16ASM\Proposta Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -78,6 +78,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="[$-816]d/mmm;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,8 +115,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -207,7 +210,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2218930959559291"/>
+          <c:y val="0.17104769139543716"/>
+          <c:w val="0.75540042513287664"/>
+          <c:h val="0.51780045196566815"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
@@ -285,7 +298,7 @@
             <c:numRef>
               <c:f>Folha1!$B$2:$B$14</c:f>
               <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
+                <c:formatCode>[$-816]d/mmm;@</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>42436</c:v>
@@ -460,11 +473,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="187084824"/>
-        <c:axId val="187079728"/>
+        <c:axId val="203392168"/>
+        <c:axId val="203387856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="187084824"/>
+        <c:axId val="203392168"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -507,7 +520,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187079728"/>
+        <c:crossAx val="203387856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -515,7 +528,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="187079728"/>
+        <c:axId val="203387856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42582"/>
@@ -537,7 +550,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:numFmt formatCode="[$-816]d/mmm;@" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -568,7 +581,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187084824"/>
+        <c:crossAx val="203392168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -1210,15 +1223,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>2294964</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>71477</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>516254</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>380502</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>52427</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1505,18 +1518,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1527,158 +1540,158 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>42436</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>42443</v>
       </c>
       <c r="C3">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>42450</v>
       </c>
       <c r="C4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>42457</v>
       </c>
       <c r="C5">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>42478</v>
       </c>
       <c r="C6">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>42485</v>
       </c>
       <c r="C7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>42492</v>
       </c>
       <c r="C8">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>42506</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>42513</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>42520</v>
       </c>
       <c r="C11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>42527</v>
       </c>
       <c r="C12">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>42541</v>
       </c>
       <c r="C13">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>42562</v>
       </c>
       <c r="C14">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="3"/>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>